<commit_message>
Benchmark article in progress
</commit_message>
<xml_diff>
--- a/development_resources/atomic-properties-benchmark-6-Jul-2018.xlsx
+++ b/development_resources/atomic-properties-benchmark-6-Jul-2018.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vadymb/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vadymb/Projects/v8tr.github.io/development_resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{1A9BFB56-D0D5-5C45-8151-1A1D84C0B972}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36FFB7B7-7B9C-E843-8A81-AB4DE3250E2B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="atomic-properties-benchmark-6-J" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,15 @@
     <sheet name="Setters" sheetId="3" r:id="rId3"/>
     <sheet name="Setter vs Getter" sheetId="4" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">'atomic-properties-benchmark-6-J'!$B$3:$B$23</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'atomic-properties-benchmark-6-J'!$C$135:$C$155</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">'atomic-properties-benchmark-6-J'!$C$179:$C$199</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">'atomic-properties-benchmark-6-J'!$C$223:$C$243</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">'atomic-properties-benchmark-6-J'!$C$3:$C$23</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">'atomic-properties-benchmark-6-J'!$C$47:$C$67</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">'atomic-properties-benchmark-6-J'!$C$91:$C$111</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -61,7 +70,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1120,67 +1129,67 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>3.5047531127929697E-7</c:v>
+                  <c:v>5.3524971008300805E-7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.49419021606445E-7</c:v>
+                  <c:v>3.38554382324219E-7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0716915130615201E-6</c:v>
+                  <c:v>5.8650970458984395E-7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.3911724090576199E-6</c:v>
+                  <c:v>1.13844871520996E-6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.5010108947753898E-6</c:v>
+                  <c:v>2.3293495178222702E-6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.4322013854980502E-6</c:v>
+                  <c:v>3.8397312164306599E-6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9.2780590057372994E-6</c:v>
+                  <c:v>9.5975399017334007E-6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.7940998077392598E-5</c:v>
+                  <c:v>1.8451213836669902E-5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.5767555236816402E-5</c:v>
+                  <c:v>3.0858516693115202E-5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7.1904659271240201E-5</c:v>
+                  <c:v>7.1291923522949201E-5</c:v>
                 </c:pt>
                 <c:pt idx="10" formatCode="General">
-                  <c:v>1.409912109375E-4</c:v>
+                  <c:v>1.53357982635498E-4</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="General">
-                  <c:v>2.8109908103942901E-4</c:v>
+                  <c:v>2.6919126510620099E-4</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="General">
-                  <c:v>5.6687951087951703E-4</c:v>
+                  <c:v>4.7912597656249998E-4</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="General">
-                  <c:v>1.1219799518585199E-3</c:v>
+                  <c:v>8.7822914123535198E-4</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="General">
-                  <c:v>2.25391864776611E-3</c:v>
+                  <c:v>1.7506289482116699E-3</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="General">
-                  <c:v>4.5566642284393302E-3</c:v>
+                  <c:v>3.4813475608825701E-3</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="General">
-                  <c:v>9.1634309291839609E-3</c:v>
+                  <c:v>7.1696853637695304E-3</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="General">
-                  <c:v>1.8224624395370499E-2</c:v>
+                  <c:v>1.40391504764557E-2</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="General">
-                  <c:v>3.6743843555450399E-2</c:v>
+                  <c:v>2.8126274347305299E-2</c:v>
                 </c:pt>
                 <c:pt idx="19" formatCode="General">
-                  <c:v>7.4641734361648601E-2</c:v>
+                  <c:v>5.57826066017151E-2</c:v>
                 </c:pt>
                 <c:pt idx="20" formatCode="General">
-                  <c:v>0.14644855737686199</c:v>
+                  <c:v>0.112635484933853</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1430,6 +1439,61 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Iterations, count</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1481,6 +1545,61 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time, s</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="#,##0" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1791,67 +1910,67 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>3.5047531127929697E-7</c:v>
+                  <c:v>5.3524971008300805E-7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.49419021606445E-7</c:v>
+                  <c:v>3.38554382324219E-7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0716915130615201E-6</c:v>
+                  <c:v>5.8650970458984395E-7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.3911724090576199E-6</c:v>
+                  <c:v>1.13844871520996E-6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.5010108947753898E-6</c:v>
+                  <c:v>2.3293495178222702E-6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.4322013854980502E-6</c:v>
+                  <c:v>3.8397312164306599E-6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9.2780590057372994E-6</c:v>
+                  <c:v>9.5975399017334007E-6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.7940998077392598E-5</c:v>
+                  <c:v>1.8451213836669902E-5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.5767555236816402E-5</c:v>
+                  <c:v>3.0858516693115202E-5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7.1904659271240201E-5</c:v>
+                  <c:v>7.1291923522949201E-5</c:v>
                 </c:pt>
                 <c:pt idx="10" formatCode="General">
-                  <c:v>1.409912109375E-4</c:v>
+                  <c:v>1.53357982635498E-4</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="General">
-                  <c:v>2.8109908103942901E-4</c:v>
+                  <c:v>2.6919126510620099E-4</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="General">
-                  <c:v>5.6687951087951703E-4</c:v>
+                  <c:v>4.7912597656249998E-4</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="General">
-                  <c:v>1.1219799518585199E-3</c:v>
+                  <c:v>8.7822914123535198E-4</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="General">
-                  <c:v>2.25391864776611E-3</c:v>
+                  <c:v>1.7506289482116699E-3</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="General">
-                  <c:v>4.5566642284393302E-3</c:v>
+                  <c:v>3.4813475608825701E-3</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="General">
-                  <c:v>9.1634309291839609E-3</c:v>
+                  <c:v>7.1696853637695304E-3</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="General">
-                  <c:v>1.8224624395370499E-2</c:v>
+                  <c:v>1.40391504764557E-2</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="General">
-                  <c:v>3.6743843555450399E-2</c:v>
+                  <c:v>2.8126274347305299E-2</c:v>
                 </c:pt>
                 <c:pt idx="19" formatCode="General">
-                  <c:v>7.4641734361648601E-2</c:v>
+                  <c:v>5.57826066017151E-2</c:v>
                 </c:pt>
                 <c:pt idx="20" formatCode="General">
-                  <c:v>0.14644855737686199</c:v>
+                  <c:v>0.112635484933853</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1900,67 +2019,67 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>1.6093254089355499E-7</c:v>
+                  <c:v>1.4781951904296899E-7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.3259391784668001E-7</c:v>
+                  <c:v>2.4795532226562501E-7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.9843063354492204E-7</c:v>
+                  <c:v>4.18424606323242E-7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.33037567138672E-6</c:v>
+                  <c:v>7.9154968261718704E-7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.4402141571044899E-6</c:v>
+                  <c:v>1.4781951904296901E-6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.3690204620361301E-6</c:v>
+                  <c:v>2.9504299163818402E-6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8.6593627929687501E-6</c:v>
+                  <c:v>5.8186054229736297E-6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.7248392105102502E-5</c:v>
+                  <c:v>1.29902362823486E-5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.4608840942382798E-5</c:v>
+                  <c:v>2.3134946823120099E-5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6.9829225540161104E-5</c:v>
-                </c:pt>
-                <c:pt idx="10" formatCode="General">
-                  <c:v>1.51020288467407E-4</c:v>
+                  <c:v>4.7906637191772502E-5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9.6278190612792994E-5</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="General">
-                  <c:v>2.9100656509399402E-4</c:v>
+                  <c:v>1.89361572265625E-4</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="General">
-                  <c:v>5.5944323539733895E-4</c:v>
+                  <c:v>3.8836240768432597E-4</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="General">
-                  <c:v>1.16571545600891E-3</c:v>
+                  <c:v>7.5763940811157204E-4</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="General">
-                  <c:v>2.28354692459106E-3</c:v>
+                  <c:v>1.5343677997589099E-3</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="General">
-                  <c:v>4.6900463104248002E-3</c:v>
+                  <c:v>3.1485438346862799E-3</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="General">
-                  <c:v>9.3674576282501195E-3</c:v>
+                  <c:v>6.2389552593231203E-3</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="General">
-                  <c:v>1.8538193702697801E-2</c:v>
+                  <c:v>1.2591866254806501E-2</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="General">
-                  <c:v>3.6584692001342803E-2</c:v>
+                  <c:v>2.51723802089691E-2</c:v>
                 </c:pt>
                 <c:pt idx="19" formatCode="General">
-                  <c:v>7.3806518316268901E-2</c:v>
+                  <c:v>4.9675164222717297E-2</c:v>
                 </c:pt>
                 <c:pt idx="20" formatCode="General">
-                  <c:v>0.150735292434692</c:v>
+                  <c:v>9.7967069149017302E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3801,67 +3920,67 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>3.5047531127929697E-7</c:v>
+                  <c:v>5.3524971008300805E-7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.49419021606445E-7</c:v>
+                  <c:v>3.38554382324219E-7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0716915130615201E-6</c:v>
+                  <c:v>5.8650970458984395E-7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.3911724090576199E-6</c:v>
+                  <c:v>1.13844871520996E-6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.5010108947753898E-6</c:v>
+                  <c:v>2.3293495178222702E-6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.4322013854980502E-6</c:v>
+                  <c:v>3.8397312164306599E-6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9.2780590057372994E-6</c:v>
+                  <c:v>9.5975399017334007E-6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.7940998077392598E-5</c:v>
+                  <c:v>1.8451213836669902E-5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.5767555236816402E-5</c:v>
+                  <c:v>3.0858516693115202E-5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7.1904659271240201E-5</c:v>
+                  <c:v>7.1291923522949201E-5</c:v>
                 </c:pt>
                 <c:pt idx="10" formatCode="General">
-                  <c:v>1.409912109375E-4</c:v>
+                  <c:v>1.53357982635498E-4</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="General">
-                  <c:v>2.8109908103942901E-4</c:v>
+                  <c:v>2.6919126510620099E-4</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="General">
-                  <c:v>5.6687951087951703E-4</c:v>
+                  <c:v>4.7912597656249998E-4</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="General">
-                  <c:v>1.1219799518585199E-3</c:v>
+                  <c:v>8.7822914123535198E-4</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="General">
-                  <c:v>2.25391864776611E-3</c:v>
+                  <c:v>1.7506289482116699E-3</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="General">
-                  <c:v>4.5566642284393302E-3</c:v>
+                  <c:v>3.4813475608825701E-3</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="General">
-                  <c:v>9.1634309291839609E-3</c:v>
+                  <c:v>7.1696853637695304E-3</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="General">
-                  <c:v>1.8224624395370499E-2</c:v>
+                  <c:v>1.40391504764557E-2</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="General">
-                  <c:v>3.6743843555450399E-2</c:v>
+                  <c:v>2.8126274347305299E-2</c:v>
                 </c:pt>
                 <c:pt idx="19" formatCode="General">
-                  <c:v>7.4641734361648601E-2</c:v>
+                  <c:v>5.57826066017151E-2</c:v>
                 </c:pt>
                 <c:pt idx="20" formatCode="General">
-                  <c:v>0.14644855737686199</c:v>
+                  <c:v>0.112635484933853</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3893,6 +4012,61 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Iterations, count</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3944,6 +4118,61 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time, s</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -4388,6 +4617,61 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Iterations, count</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -4439,6 +4723,61 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time, s</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="#,##0" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -5076,67 +5415,67 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>1.6093254089355499E-7</c:v>
+                  <c:v>1.4781951904296899E-7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.3259391784668001E-7</c:v>
+                  <c:v>2.4795532226562501E-7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.9843063354492204E-7</c:v>
+                  <c:v>4.18424606323242E-7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.33037567138672E-6</c:v>
+                  <c:v>7.9154968261718704E-7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.4402141571044899E-6</c:v>
+                  <c:v>1.4781951904296901E-6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.3690204620361301E-6</c:v>
+                  <c:v>2.9504299163818402E-6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8.6593627929687501E-6</c:v>
+                  <c:v>5.8186054229736297E-6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.7248392105102502E-5</c:v>
+                  <c:v>1.29902362823486E-5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.4608840942382798E-5</c:v>
+                  <c:v>2.3134946823120099E-5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6.9829225540161104E-5</c:v>
-                </c:pt>
-                <c:pt idx="10" formatCode="General">
-                  <c:v>1.51020288467407E-4</c:v>
+                  <c:v>4.7906637191772502E-5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9.6278190612792994E-5</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="General">
-                  <c:v>2.9100656509399402E-4</c:v>
+                  <c:v>1.89361572265625E-4</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="General">
-                  <c:v>5.5944323539733895E-4</c:v>
+                  <c:v>3.8836240768432597E-4</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="General">
-                  <c:v>1.16571545600891E-3</c:v>
+                  <c:v>7.5763940811157204E-4</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="General">
-                  <c:v>2.28354692459106E-3</c:v>
+                  <c:v>1.5343677997589099E-3</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="General">
-                  <c:v>4.6900463104248002E-3</c:v>
+                  <c:v>3.1485438346862799E-3</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="General">
-                  <c:v>9.3674576282501195E-3</c:v>
+                  <c:v>6.2389552593231203E-3</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="General">
-                  <c:v>1.8538193702697801E-2</c:v>
+                  <c:v>1.2591866254806501E-2</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="General">
-                  <c:v>3.6584692001342803E-2</c:v>
+                  <c:v>2.51723802089691E-2</c:v>
                 </c:pt>
                 <c:pt idx="19" formatCode="General">
-                  <c:v>7.3806518316268901E-2</c:v>
+                  <c:v>4.9675164222717297E-2</c:v>
                 </c:pt>
                 <c:pt idx="20" formatCode="General">
-                  <c:v>0.150735292434692</c:v>
+                  <c:v>9.7967069149017302E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6074,67 +6413,67 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>1.6093254089355499E-7</c:v>
+                  <c:v>1.4781951904296899E-7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.3259391784668001E-7</c:v>
+                  <c:v>2.4795532226562501E-7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.9843063354492204E-7</c:v>
+                  <c:v>4.18424606323242E-7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.33037567138672E-6</c:v>
+                  <c:v>7.9154968261718704E-7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.4402141571044899E-6</c:v>
+                  <c:v>1.4781951904296901E-6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.3690204620361301E-6</c:v>
+                  <c:v>2.9504299163818402E-6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8.6593627929687501E-6</c:v>
+                  <c:v>5.8186054229736297E-6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.7248392105102502E-5</c:v>
+                  <c:v>1.29902362823486E-5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.4608840942382798E-5</c:v>
+                  <c:v>2.3134946823120099E-5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6.9829225540161104E-5</c:v>
-                </c:pt>
-                <c:pt idx="10" formatCode="General">
-                  <c:v>1.51020288467407E-4</c:v>
+                  <c:v>4.7906637191772502E-5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9.6278190612792994E-5</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="General">
-                  <c:v>2.9100656509399402E-4</c:v>
+                  <c:v>1.89361572265625E-4</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="General">
-                  <c:v>5.5944323539733895E-4</c:v>
+                  <c:v>3.8836240768432597E-4</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="General">
-                  <c:v>1.16571545600891E-3</c:v>
+                  <c:v>7.5763940811157204E-4</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="General">
-                  <c:v>2.28354692459106E-3</c:v>
+                  <c:v>1.5343677997589099E-3</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="General">
-                  <c:v>4.6900463104248002E-3</c:v>
+                  <c:v>3.1485438346862799E-3</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="General">
-                  <c:v>9.3674576282501195E-3</c:v>
+                  <c:v>6.2389552593231203E-3</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="General">
-                  <c:v>1.8538193702697801E-2</c:v>
+                  <c:v>1.2591866254806501E-2</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="General">
-                  <c:v>3.6584692001342803E-2</c:v>
+                  <c:v>2.51723802089691E-2</c:v>
                 </c:pt>
                 <c:pt idx="19" formatCode="General">
-                  <c:v>7.3806518316268901E-2</c:v>
+                  <c:v>4.9675164222717297E-2</c:v>
                 </c:pt>
                 <c:pt idx="20" formatCode="General">
-                  <c:v>0.150735292434692</c:v>
+                  <c:v>9.7967069149017302E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -15042,10 +15381,10 @@
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>774700</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>787400</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -15799,11 +16138,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C264"/>
   <sheetViews>
-    <sheetView topLeftCell="A237" workbookViewId="0">
-      <selection activeCell="C112" sqref="C112"/>
+    <sheetView topLeftCell="A151" workbookViewId="0">
+      <selection activeCell="E140" sqref="E140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17241,7 +17580,7 @@
         <v>1</v>
       </c>
       <c r="C135" s="1">
-        <v>3.5047531127929697E-7</v>
+        <v>5.3524971008300805E-7</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.2">
@@ -17252,7 +17591,7 @@
         <v>2</v>
       </c>
       <c r="C136" s="1">
-        <v>4.49419021606445E-7</v>
+        <v>3.38554382324219E-7</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.2">
@@ -17263,7 +17602,7 @@
         <v>4</v>
       </c>
       <c r="C137" s="1">
-        <v>1.0716915130615201E-6</v>
+        <v>5.8650970458984395E-7</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.2">
@@ -17274,7 +17613,7 @@
         <v>8</v>
       </c>
       <c r="C138" s="1">
-        <v>1.3911724090576199E-6</v>
+        <v>1.13844871520996E-6</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.2">
@@ -17285,7 +17624,7 @@
         <v>16</v>
       </c>
       <c r="C139" s="1">
-        <v>2.5010108947753898E-6</v>
+        <v>2.3293495178222702E-6</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.2">
@@ -17296,7 +17635,7 @@
         <v>32</v>
       </c>
       <c r="C140" s="1">
-        <v>4.4322013854980502E-6</v>
+        <v>3.8397312164306599E-6</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.2">
@@ -17307,7 +17646,7 @@
         <v>64</v>
       </c>
       <c r="C141" s="1">
-        <v>9.2780590057372994E-6</v>
+        <v>9.5975399017334007E-6</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.2">
@@ -17318,7 +17657,7 @@
         <v>128</v>
       </c>
       <c r="C142" s="1">
-        <v>1.7940998077392598E-5</v>
+        <v>1.8451213836669902E-5</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.2">
@@ -17329,7 +17668,7 @@
         <v>256</v>
       </c>
       <c r="C143" s="1">
-        <v>3.5767555236816402E-5</v>
+        <v>3.0858516693115202E-5</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.2">
@@ -17340,7 +17679,7 @@
         <v>512</v>
       </c>
       <c r="C144" s="1">
-        <v>7.1904659271240201E-5</v>
+        <v>7.1291923522949201E-5</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.2">
@@ -17351,7 +17690,7 @@
         <v>1024</v>
       </c>
       <c r="C145">
-        <v>1.409912109375E-4</v>
+        <v>1.53357982635498E-4</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.2">
@@ -17362,7 +17701,7 @@
         <v>2048</v>
       </c>
       <c r="C146">
-        <v>2.8109908103942901E-4</v>
+        <v>2.6919126510620099E-4</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.2">
@@ -17373,7 +17712,7 @@
         <v>4096</v>
       </c>
       <c r="C147">
-        <v>5.6687951087951703E-4</v>
+        <v>4.7912597656249998E-4</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.2">
@@ -17384,7 +17723,7 @@
         <v>8192</v>
       </c>
       <c r="C148">
-        <v>1.1219799518585199E-3</v>
+        <v>8.7822914123535198E-4</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.2">
@@ -17395,7 +17734,7 @@
         <v>16384</v>
       </c>
       <c r="C149">
-        <v>2.25391864776611E-3</v>
+        <v>1.7506289482116699E-3</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.2">
@@ -17406,7 +17745,7 @@
         <v>32768</v>
       </c>
       <c r="C150">
-        <v>4.5566642284393302E-3</v>
+        <v>3.4813475608825701E-3</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.2">
@@ -17417,7 +17756,7 @@
         <v>65536</v>
       </c>
       <c r="C151">
-        <v>9.1634309291839609E-3</v>
+        <v>7.1696853637695304E-3</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.2">
@@ -17428,7 +17767,7 @@
         <v>131072</v>
       </c>
       <c r="C152">
-        <v>1.8224624395370499E-2</v>
+        <v>1.40391504764557E-2</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.2">
@@ -17439,7 +17778,7 @@
         <v>262144</v>
       </c>
       <c r="C153">
-        <v>3.6743843555450399E-2</v>
+        <v>2.8126274347305299E-2</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.2">
@@ -17450,7 +17789,7 @@
         <v>524288</v>
       </c>
       <c r="C154">
-        <v>7.4641734361648601E-2</v>
+        <v>5.57826066017151E-2</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.2">
@@ -17461,7 +17800,7 @@
         <v>1048576</v>
       </c>
       <c r="C155">
-        <v>0.14644855737686199</v>
+        <v>0.112635484933853</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.2">
@@ -17472,7 +17811,7 @@
         <v>1</v>
       </c>
       <c r="C156" s="1">
-        <v>1.6093254089355499E-7</v>
+        <v>1.4781951904296899E-7</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.2">
@@ -17483,7 +17822,7 @@
         <v>2</v>
       </c>
       <c r="C157" s="1">
-        <v>3.3259391784668001E-7</v>
+        <v>2.4795532226562501E-7</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.2">
@@ -17494,7 +17833,7 @@
         <v>4</v>
       </c>
       <c r="C158" s="1">
-        <v>5.9843063354492204E-7</v>
+        <v>4.18424606323242E-7</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.2">
@@ -17505,7 +17844,7 @@
         <v>8</v>
       </c>
       <c r="C159" s="1">
-        <v>1.33037567138672E-6</v>
+        <v>7.9154968261718704E-7</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.2">
@@ -17516,7 +17855,7 @@
         <v>16</v>
       </c>
       <c r="C160" s="1">
-        <v>2.4402141571044899E-6</v>
+        <v>1.4781951904296901E-6</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.2">
@@ -17527,7 +17866,7 @@
         <v>32</v>
       </c>
       <c r="C161" s="1">
-        <v>4.3690204620361301E-6</v>
+        <v>2.9504299163818402E-6</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.2">
@@ -17538,7 +17877,7 @@
         <v>64</v>
       </c>
       <c r="C162" s="1">
-        <v>8.6593627929687501E-6</v>
+        <v>5.8186054229736297E-6</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.2">
@@ -17549,7 +17888,7 @@
         <v>128</v>
       </c>
       <c r="C163" s="1">
-        <v>1.7248392105102502E-5</v>
+        <v>1.29902362823486E-5</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.2">
@@ -17560,7 +17899,7 @@
         <v>256</v>
       </c>
       <c r="C164" s="1">
-        <v>3.4608840942382798E-5</v>
+        <v>2.3134946823120099E-5</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.2">
@@ -17571,7 +17910,7 @@
         <v>512</v>
       </c>
       <c r="C165" s="1">
-        <v>6.9829225540161104E-5</v>
+        <v>4.7906637191772502E-5</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.2">
@@ -17581,8 +17920,8 @@
       <c r="B166">
         <v>1024</v>
       </c>
-      <c r="C166">
-        <v>1.51020288467407E-4</v>
+      <c r="C166" s="1">
+        <v>9.6278190612792994E-5</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.2">
@@ -17593,7 +17932,7 @@
         <v>2048</v>
       </c>
       <c r="C167">
-        <v>2.9100656509399402E-4</v>
+        <v>1.89361572265625E-4</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.2">
@@ -17604,7 +17943,7 @@
         <v>4096</v>
       </c>
       <c r="C168">
-        <v>5.5944323539733895E-4</v>
+        <v>3.8836240768432597E-4</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.2">
@@ -17615,7 +17954,7 @@
         <v>8192</v>
       </c>
       <c r="C169">
-        <v>1.16571545600891E-3</v>
+        <v>7.5763940811157204E-4</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.2">
@@ -17626,7 +17965,7 @@
         <v>16384</v>
       </c>
       <c r="C170">
-        <v>2.28354692459106E-3</v>
+        <v>1.5343677997589099E-3</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.2">
@@ -17637,7 +17976,7 @@
         <v>32768</v>
       </c>
       <c r="C171">
-        <v>4.6900463104248002E-3</v>
+        <v>3.1485438346862799E-3</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.2">
@@ -17648,7 +17987,7 @@
         <v>65536</v>
       </c>
       <c r="C172">
-        <v>9.3674576282501195E-3</v>
+        <v>6.2389552593231203E-3</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.2">
@@ -17659,7 +17998,7 @@
         <v>131072</v>
       </c>
       <c r="C173">
-        <v>1.8538193702697801E-2</v>
+        <v>1.2591866254806501E-2</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.2">
@@ -17670,7 +18009,7 @@
         <v>262144</v>
       </c>
       <c r="C174">
-        <v>3.6584692001342803E-2</v>
+        <v>2.51723802089691E-2</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.2">
@@ -17681,7 +18020,7 @@
         <v>524288</v>
       </c>
       <c r="C175">
-        <v>7.3806518316268901E-2</v>
+        <v>4.9675164222717297E-2</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.2">
@@ -17692,7 +18031,7 @@
         <v>1048576</v>
       </c>
       <c r="C176">
-        <v>0.150735292434692</v>
+        <v>9.7967069149017302E-2</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.2">
@@ -18636,22 +18975,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView topLeftCell="A57" workbookViewId="0">
@@ -18661,21 +19001,23 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="P191" sqref="P191"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>